<commit_message>
Q3 till Q6 done
</commit_message>
<xml_diff>
--- a/Homework B- Bitcoin.xlsx
+++ b/Homework B- Bitcoin.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
     <sheet name="Q2" sheetId="2" r:id="rId2"/>
+    <sheet name="Q3" sheetId="3" r:id="rId3"/>
+    <sheet name="Q4" sheetId="4" r:id="rId4"/>
+    <sheet name="Q5" sheetId="5" r:id="rId5"/>
+    <sheet name="Q6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>There are currently almost 16 million bitcoins available</t>
   </si>
@@ -65,13 +69,118 @@
   </si>
   <si>
     <t>However, in the world, spendable unit will be considered as the lowest denomination of the weakest currency which is Vietnamese Dong. 1 USD is 22376 Vietnamese Dong. Hence, spendable unit in world is 80trillion multiplied by 22376 which is much higher than available satoshis. Therefore, to answer if bitcoin can be used as global currency we need to know what are we comparing it with.</t>
+  </si>
+  <si>
+    <t>Current block height is around 436700</t>
+  </si>
+  <si>
+    <t>Number of blocks in blockchain</t>
+  </si>
+  <si>
+    <t>A block is currently limited to 1MB in size</t>
+  </si>
+  <si>
+    <t>Size of a block in MB</t>
+  </si>
+  <si>
+    <t>Size of blockchain in MB</t>
+  </si>
+  <si>
+    <t>What's the market capitalization of bitcoin as measured in US $ ?</t>
+  </si>
+  <si>
+    <t>Number of Bitcoins in circulation</t>
+  </si>
+  <si>
+    <t>Bitcoin currently trades at almost $700 for 1 bitcoin</t>
+  </si>
+  <si>
+    <t>Cost of 1 bitcoin in USD</t>
+  </si>
+  <si>
+    <t>Total cost of bitcoins</t>
+  </si>
+  <si>
+    <t>Market capitalization of Bitcoin is 11.2 billion USD</t>
+  </si>
+  <si>
+    <t>a) How many bitcoin spendable units are there currently? b) How does that compare with spendable units available in the world economy today? This is like asking: "could bitcoin be used as a global currency?"</t>
+  </si>
+  <si>
+    <t>What's the current size of the bitcoin blockchain? How quickly is it growing?</t>
+  </si>
+  <si>
+    <t>What does the blockchain verification cycle say about how quickly transactions can be verified?</t>
+  </si>
+  <si>
+    <t>A block is mined every 10 minutes on average</t>
+  </si>
+  <si>
+    <t>Time to add 1 block in blockchain (in minutes)</t>
+  </si>
+  <si>
+    <t>Rate of increase in size</t>
+  </si>
+  <si>
+    <t>1 MB per 10 minutes</t>
+  </si>
+  <si>
+    <t>We can say that the size of bitcoin blockchain is increasing at the rate of 1666.67 bytes per second (10^6 bytes per 10*60 seconds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hence, the current size of bitcoin blockchain must be 436700 MB or (436700/1024) 426.46 GB. However, the maximum block size limit has changed periodically and it was not 1 MB since its inception. Because of that the actual blockchain size is much less than what is mentioned above. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accordingly to the blockchain verification cycle, a transaction can be verified once it is permanently in main blockchain. Since a transaction can be rolled over which will avoid it from being in the main blockchain, a transaction is said to be permanently in main blockchain once 6 more blocks have been added to the blockchain after the block in which the transaction is. The number of blocks to be added for a transaction to be permanently added is defined as 6 blocks as by then the risk or chance of it getting rolled over becomes too less. </t>
+  </si>
+  <si>
+    <t>6 blocks must be added to blockchain for a transaction to be permanently added</t>
+  </si>
+  <si>
+    <t>No. of blocks to be added</t>
+  </si>
+  <si>
+    <t>Time taken for 1 block to be added (in minutes)</t>
+  </si>
+  <si>
+    <t>Total time to add 6 blocks</t>
+  </si>
+  <si>
+    <t>It takes 60 minutes to add 6 blocks to the blockchain, hence a transaction is verified in 60 minutes</t>
+  </si>
+  <si>
+    <t>What's the theoretical maximum transaction throughput of the bitcoin payments network?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction throughput can be defined as the number of transactions processed per second. </t>
+  </si>
+  <si>
+    <t>A transaction is, on average, 500 bytes in size</t>
+  </si>
+  <si>
+    <t>Block size in bytes</t>
+  </si>
+  <si>
+    <t>Time to mine a block in seconds</t>
+  </si>
+  <si>
+    <t>Size of a transaction in bytes</t>
+  </si>
+  <si>
+    <t>Maximum number of transactions in a block</t>
+  </si>
+  <si>
+    <t>Transaction throughput</t>
+  </si>
+  <si>
+    <t>Theoretical maximum transaction throughput of the bitcoin payments network is 3.5 transactions per second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,13 +210,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,7 +247,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -129,8 +257,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,22 +286,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,116 +696,350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="61.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="43" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="20">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="20">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="5">
         <f xml:space="preserve"> 16* 10^6</f>
         <v>16000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:3" ht="20">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="20">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
-        <f>C2*10^8</f>
+      <c r="C6" s="9">
+        <f>C4*10^8</f>
         <v>1600000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:3" ht="20">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
-        <f>C4</f>
+      <c r="C7" s="9">
+        <f>C6</f>
         <v>1600000000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="2" t="s">
+    <row r="8" spans="1:3" ht="20">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="20">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" s="9">
         <f>80* 10^12</f>
         <v>80000000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:3" ht="20">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3">
-        <f>C5-C7</f>
+      <c r="C10" s="9">
+        <f>C7-C9</f>
         <v>1520000000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="37" customHeight="1">
-      <c r="B9" s="4" t="s">
+    <row r="11" spans="1:3" ht="47" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" ht="110" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="53.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="51.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>436700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <f>C4*C5</f>
+        <v>436700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="101" customHeight="1">
+      <c r="B8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43" customHeight="1">
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="63.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="20">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="127" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="5" spans="1:3" ht="20">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="40">
+      <c r="A6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="40">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C6*C7</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="77" customHeight="1">
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4"/>
+    <row r="10" spans="1:3" ht="66" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -620,4 +1050,225 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20">
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="20">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="20">
+      <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="20">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="20">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4">
+        <f>1*1024*1024</f>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20">
+      <c r="A7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="40">
+      <c r="B8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C6/C7</f>
+        <v>2097.152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4">
+        <f>10*60</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4">
+        <f>C8/C9</f>
+        <v>3.4952533333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="61" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="20">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="20">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="C9" formula="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="72.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <f>16*10^6</f>
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4">
+        <f>C4*C5</f>
+        <v>11200000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>